<commit_message>
Makes the CSV readable again
</commit_message>
<xml_diff>
--- a/Thai Vehicle Stats.xlsx
+++ b/Thai Vehicle Stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="901" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="901" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RAW Data (LOCKED)" sheetId="3" r:id="rId1"/>
@@ -1291,15 +1291,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="9" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1309,6 +1300,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1405,7 +1405,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1494,11 +1493,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="497008768"/>
-        <c:axId val="497009160"/>
+        <c:axId val="317708144"/>
+        <c:axId val="317702656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497008768"/>
+        <c:axId val="317708144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497009160"/>
+        <c:crossAx val="317702656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1549,7 +1548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497009160"/>
+        <c:axId val="317702656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1600,7 +1599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497008768"/>
+        <c:crossAx val="317708144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1702,7 +1701,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1836,11 +1834,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="497040912"/>
-        <c:axId val="497038560"/>
+        <c:axId val="317703048"/>
+        <c:axId val="317705400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497040912"/>
+        <c:axId val="317703048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1883,7 +1881,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497038560"/>
+        <c:crossAx val="317705400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1891,7 +1889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497038560"/>
+        <c:axId val="317705400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,7 +1940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497040912"/>
+        <c:crossAx val="317703048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2006,7 +2004,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2132,11 +2129,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="381708840"/>
-        <c:axId val="381705704"/>
+        <c:axId val="317705792"/>
+        <c:axId val="272939064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="381708840"/>
+        <c:axId val="317705792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2179,7 +2176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381705704"/>
+        <c:crossAx val="272939064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2187,7 +2184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381705704"/>
+        <c:axId val="272939064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2238,7 +2235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381708840"/>
+        <c:crossAx val="317705792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2302,7 +2299,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2500,11 +2496,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="497009552"/>
-        <c:axId val="497005240"/>
+        <c:axId val="383736424"/>
+        <c:axId val="383736032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497009552"/>
+        <c:axId val="383736424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2547,7 +2543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497005240"/>
+        <c:crossAx val="383736032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2555,7 +2551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497005240"/>
+        <c:axId val="383736032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2606,7 +2602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497009552"/>
+        <c:crossAx val="383736424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2850,11 +2846,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="480791104"/>
-        <c:axId val="480793064"/>
+        <c:axId val="383738384"/>
+        <c:axId val="383741520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="480791104"/>
+        <c:axId val="383738384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2897,7 +2893,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480793064"/>
+        <c:crossAx val="383741520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2905,7 +2901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="480793064"/>
+        <c:axId val="383741520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2956,7 +2952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480791104"/>
+        <c:crossAx val="383738384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3020,7 +3016,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3146,11 +3141,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="486785368"/>
-        <c:axId val="486779488"/>
+        <c:axId val="383736816"/>
+        <c:axId val="383734856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="486785368"/>
+        <c:axId val="383736816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3193,7 +3188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="486779488"/>
+        <c:crossAx val="383734856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3201,7 +3196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="486779488"/>
+        <c:axId val="383734856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3252,7 +3247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="486785368"/>
+        <c:crossAx val="383736816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3478,11 +3473,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="486793992"/>
-        <c:axId val="486794776"/>
+        <c:axId val="383737208"/>
+        <c:axId val="383737600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="486793992"/>
+        <c:axId val="383737208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3525,7 +3520,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="486794776"/>
+        <c:crossAx val="383737600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3533,7 +3528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="486794776"/>
+        <c:axId val="383737600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3584,7 +3579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="486793992"/>
+        <c:crossAx val="383737208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7946,7 +7941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="BQ1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="BI1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BV4" sqref="BV4:CI6"/>
     </sheetView>
   </sheetViews>
@@ -7963,31 +7958,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:87" s="1" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="195" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
     </row>
     <row r="2" spans="1:87" s="1" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="192" t="s">
+      <c r="A2" s="196" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
+      <c r="B2" s="196"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="193" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="193"/>
-      <c r="C3" s="193"/>
-      <c r="D3" s="193"/>
+      <c r="A3" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -16112,8 +16107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:J2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -16144,523 +16139,523 @@
     <col min="76" max="87" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="194" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="194" t="s">
+    <row r="1" spans="1:87" s="191" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="191" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="194" t="s">
+      <c r="B1" s="191" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="194" t="s">
+      <c r="C1" s="191" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="194" t="s">
+      <c r="D1" s="191" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="194" t="s">
+      <c r="E1" s="191" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="194" t="s">
+      <c r="F1" s="191" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="194" t="s">
+      <c r="G1" s="191" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="194" t="s">
+      <c r="H1" s="191" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="194" t="s">
+      <c r="I1" s="191" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="194" t="s">
+      <c r="J1" s="191" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="194" t="s">
+      <c r="K1" s="191" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="194" t="s">
+      <c r="L1" s="191" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="194" t="s">
+      <c r="M1" s="191" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="194" t="s">
+      <c r="N1" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="194" t="s">
+      <c r="O1" s="191" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="194" t="s">
+      <c r="P1" s="191" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="194" t="s">
+      <c r="Q1" s="191" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="194" t="s">
+      <c r="R1" s="191" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="194" t="s">
+      <c r="S1" s="191" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="194" t="s">
+      <c r="T1" s="191" t="s">
         <v>60</v>
       </c>
-      <c r="U1" s="194" t="s">
+      <c r="U1" s="191" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="194" t="s">
+      <c r="V1" s="191" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="194" t="s">
+      <c r="W1" s="191" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="194" t="s">
+      <c r="X1" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="Y1" s="194" t="s">
+      <c r="Y1" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="Z1" s="194" t="s">
+      <c r="Z1" s="191" t="s">
         <v>66</v>
       </c>
-      <c r="AA1" s="194" t="s">
+      <c r="AA1" s="191" t="s">
         <v>67</v>
       </c>
-      <c r="AB1" s="194" t="s">
+      <c r="AB1" s="191" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" s="194" t="s">
+      <c r="AC1" s="191" t="s">
         <v>79</v>
       </c>
-      <c r="AD1" s="194" t="s">
+      <c r="AD1" s="191" t="s">
         <v>80</v>
       </c>
-      <c r="AE1" s="194" t="s">
+      <c r="AE1" s="191" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" s="194" t="s">
+      <c r="AF1" s="191" t="s">
         <v>82</v>
       </c>
-      <c r="AG1" s="194" t="s">
+      <c r="AG1" s="191" t="s">
         <v>83</v>
       </c>
-      <c r="AH1" s="194" t="s">
+      <c r="AH1" s="191" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="194" t="s">
+      <c r="AI1" s="191" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" s="194" t="s">
+      <c r="AJ1" s="191" t="s">
         <v>86</v>
       </c>
-      <c r="AK1" s="194" t="s">
+      <c r="AK1" s="191" t="s">
         <v>202</v>
       </c>
-      <c r="AL1" s="194" t="s">
+      <c r="AL1" s="191" t="s">
         <v>87</v>
       </c>
-      <c r="AM1" s="194" t="s">
+      <c r="AM1" s="191" t="s">
         <v>88</v>
       </c>
-      <c r="AN1" s="194" t="s">
+      <c r="AN1" s="191" t="s">
         <v>89</v>
       </c>
-      <c r="AO1" s="194" t="s">
+      <c r="AO1" s="191" t="s">
         <v>90</v>
       </c>
-      <c r="AP1" s="194" t="s">
+      <c r="AP1" s="191" t="s">
         <v>91</v>
       </c>
-      <c r="AQ1" s="194" t="s">
+      <c r="AQ1" s="191" t="s">
         <v>92</v>
       </c>
-      <c r="AR1" s="194" t="s">
+      <c r="AR1" s="191" t="s">
         <v>93</v>
       </c>
-      <c r="AS1" s="194" t="s">
+      <c r="AS1" s="191" t="s">
         <v>94</v>
       </c>
-      <c r="AT1" s="194" t="s">
+      <c r="AT1" s="191" t="s">
         <v>95</v>
       </c>
-      <c r="AU1" s="194" t="s">
+      <c r="AU1" s="191" t="s">
         <v>96</v>
       </c>
-      <c r="AV1" s="194" t="s">
+      <c r="AV1" s="191" t="s">
         <v>118</v>
       </c>
-      <c r="AW1" s="194" t="s">
+      <c r="AW1" s="191" t="s">
         <v>119</v>
       </c>
-      <c r="AX1" s="194" t="s">
+      <c r="AX1" s="191" t="s">
         <v>120</v>
       </c>
-      <c r="AY1" s="194" t="s">
+      <c r="AY1" s="191" t="s">
         <v>121</v>
       </c>
-      <c r="AZ1" s="194" t="s">
+      <c r="AZ1" s="191" t="s">
         <v>122</v>
       </c>
-      <c r="BA1" s="194" t="s">
+      <c r="BA1" s="191" t="s">
         <v>123</v>
       </c>
-      <c r="BB1" s="194" t="s">
+      <c r="BB1" s="191" t="s">
         <v>124</v>
       </c>
-      <c r="BC1" s="194" t="s">
+      <c r="BC1" s="191" t="s">
         <v>125</v>
       </c>
-      <c r="BD1" s="194" t="s">
+      <c r="BD1" s="191" t="s">
         <v>126</v>
       </c>
-      <c r="BE1" s="194" t="s">
+      <c r="BE1" s="191" t="s">
         <v>127</v>
       </c>
-      <c r="BF1" s="194" t="s">
+      <c r="BF1" s="191" t="s">
         <v>128</v>
       </c>
-      <c r="BG1" s="194" t="s">
+      <c r="BG1" s="191" t="s">
         <v>129</v>
       </c>
-      <c r="BH1" s="194" t="s">
+      <c r="BH1" s="191" t="s">
         <v>130</v>
       </c>
-      <c r="BI1" s="194" t="s">
+      <c r="BI1" s="191" t="s">
         <v>131</v>
       </c>
-      <c r="BJ1" s="194" t="s">
+      <c r="BJ1" s="191" t="s">
         <v>132</v>
       </c>
-      <c r="BK1" s="194" t="s">
+      <c r="BK1" s="191" t="s">
         <v>133</v>
       </c>
-      <c r="BL1" s="194" t="s">
+      <c r="BL1" s="191" t="s">
         <v>134</v>
       </c>
-      <c r="BM1" s="194" t="s">
+      <c r="BM1" s="191" t="s">
         <v>154</v>
       </c>
-      <c r="BN1" s="194" t="s">
+      <c r="BN1" s="191" t="s">
         <v>155</v>
       </c>
-      <c r="BO1" s="194" t="s">
+      <c r="BO1" s="191" t="s">
         <v>156</v>
       </c>
-      <c r="BP1" s="194" t="s">
+      <c r="BP1" s="191" t="s">
         <v>157</v>
       </c>
-      <c r="BQ1" s="194" t="s">
+      <c r="BQ1" s="191" t="s">
         <v>158</v>
       </c>
-      <c r="BR1" s="194" t="s">
+      <c r="BR1" s="191" t="s">
         <v>159</v>
       </c>
-      <c r="BS1" s="194" t="s">
+      <c r="BS1" s="191" t="s">
         <v>160</v>
       </c>
-      <c r="BT1" s="194" t="s">
+      <c r="BT1" s="191" t="s">
         <v>161</v>
       </c>
-      <c r="BV1" s="194" t="s">
+      <c r="BV1" s="191" t="s">
         <v>172</v>
       </c>
-      <c r="BW1" s="194" t="s">
+      <c r="BW1" s="191" t="s">
         <v>173</v>
       </c>
-      <c r="BX1" s="194" t="s">
+      <c r="BX1" s="191" t="s">
         <v>174</v>
       </c>
-      <c r="BY1" s="194" t="s">
+      <c r="BY1" s="191" t="s">
         <v>175</v>
       </c>
-      <c r="BZ1" s="194" t="s">
+      <c r="BZ1" s="191" t="s">
         <v>176</v>
       </c>
-      <c r="CA1" s="194" t="s">
+      <c r="CA1" s="191" t="s">
         <v>177</v>
       </c>
-      <c r="CB1" s="194" t="s">
+      <c r="CB1" s="191" t="s">
         <v>178</v>
       </c>
-      <c r="CC1" s="194" t="s">
+      <c r="CC1" s="191" t="s">
         <v>179</v>
       </c>
-      <c r="CD1" s="194" t="s">
+      <c r="CD1" s="191" t="s">
         <v>180</v>
       </c>
-      <c r="CE1" s="194" t="s">
+      <c r="CE1" s="191" t="s">
         <v>181</v>
       </c>
-      <c r="CF1" s="194" t="s">
+      <c r="CF1" s="191" t="s">
         <v>182</v>
       </c>
-      <c r="CG1" s="194" t="s">
+      <c r="CG1" s="191" t="s">
         <v>183</v>
       </c>
-      <c r="CH1" s="194" t="s">
+      <c r="CH1" s="191" t="s">
         <v>184</v>
       </c>
-      <c r="CI1" s="194" t="s">
+      <c r="CI1" s="191" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:87" s="195" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="195" t="s">
+    <row r="2" spans="1:87" s="192" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="195">
+      <c r="B2" s="192">
         <v>37120948</v>
       </c>
-      <c r="C2" s="195">
+      <c r="C2" s="192">
         <v>27885586</v>
       </c>
-      <c r="D2" s="195">
+      <c r="D2" s="192">
         <v>9235362</v>
       </c>
-      <c r="E2" s="195">
+      <c r="E2" s="192">
         <v>2170767</v>
       </c>
-      <c r="F2" s="195">
+      <c r="F2" s="192">
         <v>11610158</v>
       </c>
-      <c r="G2" s="195">
+      <c r="G2" s="192">
         <v>8019217</v>
       </c>
-      <c r="H2" s="195">
+      <c r="H2" s="192">
         <v>6646933</v>
       </c>
-      <c r="I2" s="195">
+      <c r="I2" s="192">
         <v>2771924</v>
       </c>
-      <c r="J2" s="195">
+      <c r="J2" s="192">
         <v>4675162</v>
       </c>
-      <c r="K2" s="195">
+      <c r="K2" s="192">
         <v>172429</v>
       </c>
-      <c r="L2" s="195">
+      <c r="L2" s="192">
         <v>135628</v>
       </c>
-      <c r="M2" s="195">
+      <c r="M2" s="192">
         <v>412002</v>
       </c>
-      <c r="N2" s="195">
+      <c r="N2" s="192">
         <v>150409</v>
       </c>
-      <c r="O2" s="195">
+      <c r="O2" s="192">
         <v>416705</v>
       </c>
-      <c r="P2" s="195">
+      <c r="P2" s="192">
         <v>416328</v>
       </c>
-      <c r="Q2" s="195">
+      <c r="Q2" s="192">
         <v>144507</v>
       </c>
-      <c r="R2" s="195">
+      <c r="R2" s="192">
         <v>182045</v>
       </c>
-      <c r="S2" s="195">
+      <c r="S2" s="192">
         <v>144614</v>
       </c>
-      <c r="T2" s="195">
+      <c r="T2" s="192">
         <v>123291</v>
       </c>
-      <c r="U2" s="195">
+      <c r="U2" s="192">
         <v>257792</v>
       </c>
-      <c r="V2" s="195">
+      <c r="V2" s="192">
         <v>378693</v>
       </c>
-      <c r="W2" s="195">
+      <c r="W2" s="192">
         <v>1432816</v>
       </c>
-      <c r="X2" s="195">
+      <c r="X2" s="192">
         <v>685357</v>
       </c>
-      <c r="Y2" s="195">
+      <c r="Y2" s="192">
         <v>362162</v>
       </c>
-      <c r="Z2" s="195">
+      <c r="Z2" s="192">
         <v>131348</v>
       </c>
-      <c r="AA2" s="195">
+      <c r="AA2" s="192">
         <v>221598</v>
       </c>
-      <c r="AB2" s="195">
+      <c r="AB2" s="192">
         <v>360326</v>
       </c>
-      <c r="AC2" s="195">
+      <c r="AC2" s="192">
         <v>203899</v>
       </c>
-      <c r="AD2" s="195">
+      <c r="AD2" s="192">
         <v>701817</v>
       </c>
-      <c r="AE2" s="195">
+      <c r="AE2" s="192">
         <v>387703</v>
       </c>
-      <c r="AF2" s="195">
+      <c r="AF2" s="192">
         <v>485829</v>
       </c>
-      <c r="AG2" s="195">
+      <c r="AG2" s="192">
         <v>1293523</v>
       </c>
-      <c r="AH2" s="195">
+      <c r="AH2" s="192">
         <v>444978</v>
       </c>
-      <c r="AI2" s="195">
+      <c r="AI2" s="192">
         <v>121165</v>
       </c>
-      <c r="AJ2" s="195">
+      <c r="AJ2" s="192">
         <v>154225</v>
       </c>
-      <c r="AK2" s="195">
+      <c r="AK2" s="192">
         <v>98111</v>
       </c>
-      <c r="AL2" s="195">
+      <c r="AL2" s="192">
         <v>221173</v>
       </c>
-      <c r="AM2" s="195">
+      <c r="AM2" s="192">
         <v>259646</v>
       </c>
-      <c r="AN2" s="195">
+      <c r="AN2" s="192">
         <v>645826</v>
       </c>
-      <c r="AO2" s="195">
+      <c r="AO2" s="192">
         <v>213657</v>
       </c>
-      <c r="AP2" s="195">
+      <c r="AP2" s="192">
         <v>456473</v>
       </c>
-      <c r="AQ2" s="195">
+      <c r="AQ2" s="192">
         <v>820245</v>
       </c>
-      <c r="AR2" s="195">
+      <c r="AR2" s="192">
         <v>285970</v>
       </c>
-      <c r="AS2" s="195">
+      <c r="AS2" s="192">
         <v>323476</v>
       </c>
-      <c r="AT2" s="195">
+      <c r="AT2" s="192">
         <v>387544</v>
       </c>
-      <c r="AU2" s="195">
+      <c r="AU2" s="192">
         <v>155442</v>
       </c>
-      <c r="AV2" s="195">
+      <c r="AV2" s="192">
         <v>700936</v>
       </c>
-      <c r="AW2" s="195">
+      <c r="AW2" s="192">
         <v>57536</v>
       </c>
-      <c r="AX2" s="195">
+      <c r="AX2" s="192">
         <v>1349910</v>
       </c>
-      <c r="AY2" s="195">
+      <c r="AY2" s="192">
         <v>264432</v>
       </c>
-      <c r="AZ2" s="195">
+      <c r="AZ2" s="192">
         <v>225384</v>
       </c>
-      <c r="BA2" s="195">
+      <c r="BA2" s="192">
         <v>269853</v>
       </c>
-      <c r="BB2" s="195">
+      <c r="BB2" s="192">
         <v>446759</v>
       </c>
-      <c r="BC2" s="195">
+      <c r="BC2" s="192">
         <v>253485</v>
       </c>
-      <c r="BD2" s="195">
+      <c r="BD2" s="192">
         <v>255755</v>
       </c>
-      <c r="BE2" s="195">
+      <c r="BE2" s="192">
         <v>304531</v>
       </c>
-      <c r="BF2" s="195">
+      <c r="BF2" s="192">
         <v>221147</v>
       </c>
-      <c r="BG2" s="195">
+      <c r="BG2" s="192">
         <v>480971</v>
       </c>
-      <c r="BH2" s="195">
+      <c r="BH2" s="192">
         <v>353195</v>
       </c>
-      <c r="BI2" s="195">
+      <c r="BI2" s="192">
         <v>288931</v>
       </c>
-      <c r="BJ2" s="195">
+      <c r="BJ2" s="192">
         <v>443819</v>
       </c>
-      <c r="BK2" s="195">
+      <c r="BK2" s="192">
         <v>554211</v>
       </c>
-      <c r="BL2" s="195">
+      <c r="BL2" s="192">
         <v>177562</v>
       </c>
-      <c r="BM2" s="195">
+      <c r="BM2" s="192">
         <v>481576</v>
       </c>
-      <c r="BN2" s="195">
+      <c r="BN2" s="192">
         <v>397001</v>
       </c>
-      <c r="BO2" s="195">
+      <c r="BO2" s="192">
         <v>462914</v>
       </c>
-      <c r="BP2" s="195">
+      <c r="BP2" s="192">
         <v>492523</v>
       </c>
-      <c r="BQ2" s="195">
+      <c r="BQ2" s="192">
         <v>230365</v>
       </c>
-      <c r="BR2" s="195">
+      <c r="BR2" s="192">
         <v>69583</v>
       </c>
-      <c r="BS2" s="195">
+      <c r="BS2" s="192">
         <v>315275</v>
       </c>
-      <c r="BT2" s="195">
+      <c r="BT2" s="192">
         <v>323393</v>
       </c>
-      <c r="BV2" s="195">
+      <c r="BV2" s="192">
         <v>288511</v>
       </c>
-      <c r="BW2" s="195">
+      <c r="BW2" s="192">
         <v>84644</v>
       </c>
-      <c r="BX2" s="195">
+      <c r="BX2" s="192">
         <v>597171</v>
       </c>
-      <c r="BY2" s="195">
+      <c r="BY2" s="192">
         <v>122745</v>
       </c>
-      <c r="BZ2" s="195">
+      <c r="BZ2" s="192">
         <v>617511</v>
       </c>
-      <c r="CA2" s="195">
+      <c r="CA2" s="192">
         <v>245571</v>
       </c>
-      <c r="CB2" s="195">
+      <c r="CB2" s="192">
         <v>452411</v>
       </c>
-      <c r="CC2" s="195">
+      <c r="CC2" s="192">
         <v>246757</v>
       </c>
-      <c r="CD2" s="195">
+      <c r="CD2" s="192">
         <v>354028</v>
       </c>
-      <c r="CE2" s="195">
+      <c r="CE2" s="192">
         <v>814208</v>
       </c>
-      <c r="CF2" s="195">
+      <c r="CF2" s="192">
         <v>133028</v>
       </c>
-      <c r="CG2" s="195">
+      <c r="CG2" s="192">
         <v>220058</v>
       </c>
-      <c r="CH2" s="195">
+      <c r="CH2" s="192">
         <v>266119</v>
       </c>
-      <c r="CI2" s="195">
+      <c r="CI2" s="192">
         <v>232610</v>
       </c>
     </row>
@@ -23136,58 +23131,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="196">
+      <c r="B1" s="193">
         <v>2170767</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A2" s="197" t="s">
+      <c r="A2" s="194" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="196">
+      <c r="B2" s="193">
         <v>2771924</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="194" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="196">
+      <c r="B3" s="193">
         <v>4675162</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="197" t="s">
+      <c r="A4" s="194" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="196">
+      <c r="B4" s="193">
         <v>6646933</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A5" s="197" t="s">
+      <c r="A5" s="194" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="196">
+      <c r="B5" s="193">
         <v>8019217</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="194" t="s">
         <v>201</v>
       </c>
-      <c r="B6" s="196">
+      <c r="B6" s="193">
         <v>9235362</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="194" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="196">
+      <c r="B7" s="193">
         <v>11610158</v>
       </c>
     </row>
@@ -23218,7 +23213,7 @@
       <c r="A1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="195">
+      <c r="B1" s="192">
         <v>135628</v>
       </c>
     </row>
@@ -23226,7 +23221,7 @@
       <c r="A2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="195">
+      <c r="B2" s="192">
         <v>144507</v>
       </c>
     </row>
@@ -23234,7 +23229,7 @@
       <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="195">
+      <c r="B3" s="192">
         <v>144614</v>
       </c>
     </row>
@@ -23242,7 +23237,7 @@
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="195">
+      <c r="B4" s="192">
         <v>150409</v>
       </c>
     </row>
@@ -23250,7 +23245,7 @@
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="195">
+      <c r="B5" s="192">
         <v>172429</v>
       </c>
     </row>
@@ -23258,7 +23253,7 @@
       <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="195">
+      <c r="B6" s="192">
         <v>182045</v>
       </c>
     </row>
@@ -23266,7 +23261,7 @@
       <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="195">
+      <c r="B7" s="192">
         <v>412002</v>
       </c>
     </row>
@@ -23274,7 +23269,7 @@
       <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="195">
+      <c r="B8" s="192">
         <v>416328</v>
       </c>
     </row>
@@ -23282,7 +23277,7 @@
       <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="195">
+      <c r="B9" s="192">
         <v>416705</v>
       </c>
     </row>
@@ -23799,7 +23794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>

</xml_diff>